<commit_message>
in progress. 3 tsts failing
</commit_message>
<xml_diff>
--- a/test/testdata/testSBEarningUsdc_uniqueOwner_1_deposit_1_withdr.xlsx
+++ b/test/testdata/testSBEarningUsdc_uniqueOwner_1_deposit_1_withdr.xlsx
@@ -445,7 +445,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -480,6 +480,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -797,10 +798,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K46"/>
+  <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H30" workbookViewId="0">
-      <selection activeCell="F42" sqref="E42:F46"/>
+    <sheetView tabSelected="1" topLeftCell="B29" workbookViewId="0">
+      <selection activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="25.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2165,6 +2166,12 @@
         <v>52</v>
       </c>
     </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="I47" s="12">
+        <f>SUM(I42:I46)</f>
+        <v>27.318691927599996</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A7:K7"/>

</xml_diff>